<commit_message>
Can now upload questions in X language
</commit_message>
<xml_diff>
--- a/files/offline-question-sheet.xlsx
+++ b/files/offline-question-sheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schoolofcomputingmacbook/Dropbox/Personal/pikle-productions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/pathfinder-bible-experience-engine/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE465495-CFD5-F643-820A-D2A805924351}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Type</t>
   </si>
@@ -111,12 +112,24 @@
   </si>
   <si>
     <t>Commentary Number</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Spanish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -436,26 +449,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1640625" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,46 +476,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -510,25 +526,28 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -536,34 +555,37 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>21</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
         <v>16</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
       <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -571,22 +593,25 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>16</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
       <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -594,28 +619,31 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>4</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>16</v>
       </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
       <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -623,25 +651,28 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="L6">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>4</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>16</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -649,18 +680,21 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>3</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>25</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>2</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>4</v>
       </c>
     </row>

</xml_diff>